<commit_message>
pagina web y ejercicio4
</commit_message>
<xml_diff>
--- a/ejercicio3/ejercicio3.xlsx
+++ b/ejercicio3/ejercicio3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\raices\ejercicio3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6348E4C5-3A77-4B85-8892-AD773CE39579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D4ADBC-9FF5-4DE0-ACC8-98F21D0029C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{9B82493B-48CC-4ECE-B3A9-CD54E9735952}"/>
   </bookViews>
@@ -160,8 +160,8 @@
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0000000000E+00"/>
-    <numFmt numFmtId="166" formatCode="0.00000000%"/>
-    <numFmt numFmtId="189" formatCode="0.00000%"/>
+    <numFmt numFmtId="165" formatCode="0.00000000%"/>
+    <numFmt numFmtId="166" formatCode="0.00000%"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -259,7 +259,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -283,11 +283,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -295,11 +298,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -307,10 +313,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -320,23 +326,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="189" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="2" builtinId="3"/>
@@ -374,7 +363,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>307588</xdr:colOff>
+      <xdr:colOff>307589</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>148699</xdr:rowOff>
     </xdr:to>
@@ -418,7 +407,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>453373</xdr:colOff>
+      <xdr:colOff>404212</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>92440</xdr:rowOff>
     </xdr:to>
@@ -484,7 +473,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>625842</xdr:colOff>
+      <xdr:colOff>601261</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>138546</xdr:rowOff>
     </xdr:to>
@@ -527,8 +516,8 @@
       <xdr:rowOff>131618</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="913905" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="CuadroTexto 8">
@@ -570,6 +559,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -610,7 +600,7 @@
                       <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>]=[-2,-1]</m:t>
+                      <m:t>]=[−2,−1]</m:t>
                     </m:r>
                   </m:oMath>
                 </m:oMathPara>
@@ -620,7 +610,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="CuadroTexto 8">
@@ -684,8 +674,8 @@
       <xdr:rowOff>99291</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="796757" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="CuadroTexto 9">
@@ -727,6 +717,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -777,7 +768,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="CuadroTexto 9">
@@ -841,8 +832,8 @@
       <xdr:rowOff>91594</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="796757" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="CuadroTexto 11">
@@ -884,6 +875,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -934,7 +926,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="CuadroTexto 11">
@@ -1157,8 +1149,8 @@
       <xdr:rowOff>87312</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="645305" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="CuadroTexto 5">
@@ -1200,6 +1192,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1245,7 +1238,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="CuadroTexto 5">
@@ -1309,8 +1302,8 @@
       <xdr:rowOff>80963</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="539891" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="CuadroTexto 6">
@@ -1352,6 +1345,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1403,7 +1397,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="CuadroTexto 6">
@@ -1473,8 +1467,8 @@
       <xdr:rowOff>90487</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="539891" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="CuadroTexto 7">
@@ -1516,6 +1510,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1567,7 +1562,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="CuadroTexto 7">
@@ -1637,8 +1632,8 @@
       <xdr:rowOff>70643</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2304413" cy="226152"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="CuadroTexto 8">
@@ -1680,6 +1675,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1828,7 +1824,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="CuadroTexto 8">
@@ -2063,8 +2059,8 @@
       <xdr:rowOff>131618</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="913905" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="CuadroTexto 6">
@@ -2106,6 +2102,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -2146,7 +2143,7 @@
                       <a:rPr lang="en-US" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>]=[-2,-1]</m:t>
+                      <m:t>]=[−2,−1]</m:t>
                     </m:r>
                   </m:oMath>
                 </m:oMathPara>
@@ -2156,7 +2153,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="CuadroTexto 6">
@@ -2220,8 +2217,8 @@
       <xdr:rowOff>99291</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="796757" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="CuadroTexto 7">
@@ -2263,6 +2260,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -2313,7 +2311,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="CuadroTexto 7">
@@ -2377,8 +2375,8 @@
       <xdr:rowOff>91594</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="796757" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="CuadroTexto 8">
@@ -2420,6 +2418,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -2470,7 +2469,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="CuadroTexto 8">
@@ -3534,96 +3533,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8209D4-A324-49F0-9336-02BDE4B8DD02}">
-  <dimension ref="A6:AA90"/>
+  <dimension ref="A6:O126"/>
   <sheetViews>
-    <sheetView topLeftCell="B18" zoomScale="93" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView topLeftCell="A62" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="I78" sqref="I78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11.5546875" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="18">
         <v>-1.2340932753</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="13" t="s">
+      <c r="D7" s="18"/>
+      <c r="E7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="14">
         <v>0.31546600079999998</v>
       </c>
-      <c r="G7" s="26"/>
-      <c r="H7" s="13" t="s">
+      <c r="G7" s="14"/>
+      <c r="H7" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="14">
         <v>1.7802405007</v>
       </c>
-      <c r="J7" s="26"/>
+      <c r="J7" s="14"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="13"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="14" spans="2:10" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B14" s="4" t="s">
@@ -3631,38 +3638,38 @@
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -3690,62 +3697,8 @@
       <c r="I21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J21" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="K21" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L21" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="M21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="N21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="O21" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="P21" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q21" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="R21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="S21" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T21" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="U21" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="V21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="W21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="X21" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y21" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z21" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA21" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>0</v>
       </c>
@@ -3774,73 +3727,17 @@
       <c r="I22">
         <v>1E-4</v>
       </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22">
-        <v>1</v>
-      </c>
-      <c r="N22">
-        <f t="shared" ref="N22:N36" si="2">(L22+M22)/2</f>
-        <v>0.5</v>
-      </c>
-      <c r="O22">
-        <f>L22^3-(L22^2*EXP(-0.5*L22))-3*L22+1</f>
-        <v>1</v>
-      </c>
-      <c r="P22">
-        <f t="shared" ref="P22:P36" si="3">M22^3-(M22^2*EXP(-0.5*M22))-3*M22+1</f>
-        <v>-1.6065306597126332</v>
-      </c>
-      <c r="Q22">
-        <f t="shared" ref="Q22:Q36" si="4">N22^3-(N22^2*EXP(-0.5*N22))-3*N22+1</f>
-        <v>-0.56970019576785114</v>
-      </c>
-      <c r="R22">
-        <v>1E-4</v>
-      </c>
-      <c r="T22">
-        <v>0</v>
-      </c>
-      <c r="U22">
-        <v>1</v>
-      </c>
-      <c r="V22">
-        <v>2</v>
-      </c>
-      <c r="W22">
-        <f t="shared" ref="W22:W36" si="5">(U22+V22)/2</f>
-        <v>1.5</v>
-      </c>
-      <c r="X22">
-        <f>U22^3-(U22^2*EXP(-0.5*U22))-3*U22+1</f>
-        <v>-1.6065306597126332</v>
-      </c>
-      <c r="Y22">
-        <f t="shared" ref="Y22:Y36" si="6">V22^3-(V22^2*EXP(-0.5*V22))-3*V22+1</f>
-        <v>1.5284822353142307</v>
-      </c>
-      <c r="Z22">
-        <f t="shared" ref="Z22:Z36" si="7">W22^3-(W22^2*EXP(-0.5*W22))-3*W22+1</f>
-        <v>-1.1878247436672833</v>
-      </c>
-      <c r="AA22">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23">
-        <f t="shared" ref="C23:C31" si="8">IF(F22*H22&lt;0,C22,E22)</f>
+        <f t="shared" ref="C23:C31" si="2">IF(F22*H22&lt;0,C22,E22)</f>
         <v>-1.5</v>
       </c>
       <c r="D23">
-        <f t="shared" ref="D23:D31" si="9">IF(F22*H22&lt;0,E22,D22)</f>
+        <f t="shared" ref="D23:D31" si="3">IF(F22*H22&lt;0,E22,D22)</f>
         <v>-1</v>
       </c>
       <c r="E23">
@@ -3848,82 +3745,28 @@
         <v>-1.25</v>
       </c>
       <c r="F23">
-        <f t="shared" ref="F23:F31" si="10">C23^3-(C23^2*EXP(-0.5*C23))-3*C23+1</f>
+        <f t="shared" ref="F23:F31" si="4">C23^3-(C23^2*EXP(-0.5*C23))-3*C23+1</f>
         <v>-2.6382500373785192</v>
       </c>
       <c r="G23">
-        <f t="shared" ref="G23:G31" si="11">D23^3-(D23^2*EXP(-0.5*D23))-3*D23+1</f>
+        <f t="shared" ref="G23:G31" si="5">D23^3-(D23^2*EXP(-0.5*D23))-3*D23+1</f>
         <v>1.3512787292998718</v>
       </c>
       <c r="H23">
-        <f t="shared" ref="H23:H31" si="12">E23^3-(E23^2*EXP(-0.5*E23))-3*E23+1</f>
+        <f t="shared" ref="H23:H31" si="6">E23^3-(E23^2*EXP(-0.5*E23))-3*E23+1</f>
         <v>-0.12225930848784738</v>
       </c>
-      <c r="K23">
-        <v>1</v>
-      </c>
-      <c r="L23">
-        <f t="shared" ref="L23:L36" si="13">IF(O22*Q22&lt;0,L22,N22)</f>
-        <v>0</v>
-      </c>
-      <c r="M23">
-        <f t="shared" ref="M23:M36" si="14">IF(O22*Q22&lt;0,N22,M22)</f>
-        <v>0.5</v>
-      </c>
-      <c r="N23">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="O23">
-        <f t="shared" ref="O23:O36" si="15">L23^3-(L23^2*EXP(-0.5*L23))-3*L23+1</f>
-        <v>1</v>
-      </c>
-      <c r="P23">
-        <f t="shared" si="3"/>
-        <v>-0.56970019576785114</v>
-      </c>
-      <c r="Q23">
-        <f t="shared" si="4"/>
-        <v>0.2104689435884628</v>
-      </c>
-      <c r="T23">
-        <v>1</v>
-      </c>
-      <c r="U23">
-        <f t="shared" ref="U23:U36" si="16">IF(X22*Z22&lt;0,U22,W22)</f>
-        <v>1.5</v>
-      </c>
-      <c r="V23">
-        <f t="shared" ref="V23:V36" si="17">IF(X22*Z22&lt;0,W22,V22)</f>
-        <v>2</v>
-      </c>
-      <c r="W23">
-        <f t="shared" si="5"/>
-        <v>1.75</v>
-      </c>
-      <c r="X23">
-        <f t="shared" ref="X23:X36" si="18">U23^3-(U23^2*EXP(-0.5*U23))-3*U23+1</f>
-        <v>-1.1878247436672833</v>
-      </c>
-      <c r="Y23">
-        <f t="shared" si="6"/>
-        <v>1.5284822353142307</v>
-      </c>
-      <c r="Z23">
-        <f t="shared" si="7"/>
-        <v>-0.16726493526543162</v>
-      </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>2</v>
       </c>
       <c r="C24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-1.25</v>
       </c>
       <c r="D24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>-1</v>
       </c>
       <c r="E24">
@@ -3931,82 +3774,28 @@
         <v>-1.125</v>
       </c>
       <c r="F24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>-0.12225930848784738</v>
       </c>
       <c r="G24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>1.3512787292998718</v>
       </c>
       <c r="H24">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>0.72993082478462235</v>
       </c>
-      <c r="K24">
-        <v>2</v>
-      </c>
-      <c r="L24">
-        <f t="shared" si="13"/>
-        <v>0.25</v>
-      </c>
-      <c r="M24">
-        <f t="shared" si="14"/>
-        <v>0.5</v>
-      </c>
-      <c r="N24">
-        <f t="shared" si="2"/>
-        <v>0.375</v>
-      </c>
-      <c r="O24">
-        <f t="shared" si="15"/>
-        <v>0.2104689435884628</v>
-      </c>
-      <c r="P24">
-        <f t="shared" si="3"/>
-        <v>-0.56970019576785114</v>
-      </c>
-      <c r="Q24">
-        <f t="shared" si="4"/>
-        <v>-0.18884784474411886</v>
-      </c>
-      <c r="T24">
-        <v>2</v>
-      </c>
-      <c r="U24">
-        <f t="shared" si="16"/>
-        <v>1.75</v>
-      </c>
-      <c r="V24">
-        <f t="shared" si="17"/>
-        <v>2</v>
-      </c>
-      <c r="W24">
-        <f t="shared" si="5"/>
-        <v>1.875</v>
-      </c>
-      <c r="X24">
-        <f t="shared" si="18"/>
-        <v>-0.16726493526543162</v>
-      </c>
-      <c r="Y24">
-        <f t="shared" si="6"/>
-        <v>1.5284822353142307</v>
-      </c>
-      <c r="Z24">
-        <f t="shared" si="7"/>
-        <v>0.59005834371437871</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>3</v>
       </c>
       <c r="C25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-1.25</v>
       </c>
       <c r="D25">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>-1.125</v>
       </c>
       <c r="E25">
@@ -4014,82 +3803,28 @@
         <v>-1.1875</v>
       </c>
       <c r="F25">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>-0.12225930848784738</v>
       </c>
       <c r="G25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>0.72993082478462235</v>
       </c>
       <c r="H25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>0.33447635923789498</v>
       </c>
-      <c r="K25">
-        <v>3</v>
-      </c>
-      <c r="L25">
-        <f t="shared" si="13"/>
-        <v>0.25</v>
-      </c>
-      <c r="M25">
-        <f t="shared" si="14"/>
-        <v>0.375</v>
-      </c>
-      <c r="N25">
-        <f t="shared" si="2"/>
-        <v>0.3125</v>
-      </c>
-      <c r="O25">
-        <f t="shared" si="15"/>
-        <v>0.2104689435884628</v>
-      </c>
-      <c r="P25">
-        <f t="shared" si="3"/>
-        <v>-0.18884784474411886</v>
-      </c>
-      <c r="Q25">
-        <f t="shared" si="4"/>
-        <v>9.4877610051344874E-3</v>
-      </c>
-      <c r="T25">
-        <v>3</v>
-      </c>
-      <c r="U25">
-        <f t="shared" si="16"/>
-        <v>1.75</v>
-      </c>
-      <c r="V25">
-        <f t="shared" si="17"/>
-        <v>1.875</v>
-      </c>
-      <c r="W25">
-        <f t="shared" si="5"/>
-        <v>1.8125</v>
-      </c>
-      <c r="X25">
-        <f t="shared" si="18"/>
-        <v>-0.16726493526543162</v>
-      </c>
-      <c r="Y25">
-        <f t="shared" si="6"/>
-        <v>0.59005834371437871</v>
-      </c>
-      <c r="Z25">
-        <f t="shared" si="7"/>
-        <v>0.18952259218409928</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>4</v>
       </c>
       <c r="C26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-1.25</v>
       </c>
       <c r="D26">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>-1.1875</v>
       </c>
       <c r="E26">
@@ -4097,82 +3832,28 @@
         <v>-1.21875</v>
       </c>
       <c r="F26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>-0.12225930848784738</v>
       </c>
       <c r="G26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>0.33447635923789498</v>
       </c>
       <c r="H26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>0.11399815032026517</v>
       </c>
-      <c r="K26">
-        <v>4</v>
-      </c>
-      <c r="L26">
-        <f t="shared" si="13"/>
-        <v>0.3125</v>
-      </c>
-      <c r="M26">
-        <f t="shared" si="14"/>
-        <v>0.375</v>
-      </c>
-      <c r="N26">
-        <f t="shared" si="2"/>
-        <v>0.34375</v>
-      </c>
-      <c r="O26">
-        <f t="shared" si="15"/>
-        <v>9.4877610051344874E-3</v>
-      </c>
-      <c r="P26">
-        <f t="shared" si="3"/>
-        <v>-0.18884784474411886</v>
-      </c>
-      <c r="Q26">
-        <f t="shared" si="4"/>
-        <v>-9.0135220394872428E-2</v>
-      </c>
-      <c r="T26">
-        <v>4</v>
-      </c>
-      <c r="U26">
-        <f t="shared" si="16"/>
-        <v>1.75</v>
-      </c>
-      <c r="V26">
-        <f t="shared" si="17"/>
-        <v>1.8125</v>
-      </c>
-      <c r="W26">
-        <f t="shared" si="5"/>
-        <v>1.78125</v>
-      </c>
-      <c r="X26">
-        <f t="shared" si="18"/>
-        <v>-0.16726493526543162</v>
-      </c>
-      <c r="Y26">
-        <f t="shared" si="6"/>
-        <v>0.18952259218409928</v>
-      </c>
-      <c r="Z26">
-        <f t="shared" si="7"/>
-        <v>5.7561880955994127E-3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>5</v>
       </c>
       <c r="C27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-1.25</v>
       </c>
       <c r="D27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>-1.21875</v>
       </c>
       <c r="E27">
@@ -4180,82 +3861,28 @@
         <v>-1.234375</v>
       </c>
       <c r="F27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>-0.12225930848784738</v>
       </c>
       <c r="G27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>0.11399815032026517</v>
       </c>
       <c r="H27">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>-2.1290798148916323E-3</v>
       </c>
-      <c r="K27">
-        <v>5</v>
-      </c>
-      <c r="L27">
-        <f t="shared" si="13"/>
-        <v>0.3125</v>
-      </c>
-      <c r="M27">
-        <f t="shared" si="14"/>
-        <v>0.34375</v>
-      </c>
-      <c r="N27">
-        <f t="shared" si="2"/>
-        <v>0.328125</v>
-      </c>
-      <c r="O27">
-        <f t="shared" si="15"/>
-        <v>9.4877610051344874E-3</v>
-      </c>
-      <c r="P27">
-        <f t="shared" si="3"/>
-        <v>-9.0135220394872428E-2</v>
-      </c>
-      <c r="Q27">
-        <f t="shared" si="4"/>
-        <v>-4.0422049298882712E-2</v>
-      </c>
-      <c r="T27">
-        <v>5</v>
-      </c>
-      <c r="U27">
-        <f t="shared" si="16"/>
-        <v>1.75</v>
-      </c>
-      <c r="V27">
-        <f t="shared" si="17"/>
-        <v>1.78125</v>
-      </c>
-      <c r="W27">
-        <f t="shared" si="5"/>
-        <v>1.765625</v>
-      </c>
-      <c r="X27">
-        <f t="shared" si="18"/>
-        <v>-0.16726493526543162</v>
-      </c>
-      <c r="Y27">
-        <f t="shared" si="6"/>
-        <v>5.7561880955994127E-3</v>
-      </c>
-      <c r="Z27">
-        <f t="shared" si="7"/>
-        <v>-8.2085517878812908E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>6</v>
       </c>
       <c r="C28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-1.234375</v>
       </c>
       <c r="D28">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>-1.21875</v>
       </c>
       <c r="E28">
@@ -4263,82 +3890,28 @@
         <v>-1.2265625</v>
       </c>
       <c r="F28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>-2.1290798148916323E-3</v>
       </c>
       <c r="G28">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>0.11399815032026517</v>
       </c>
       <c r="H28">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>5.6431254909981021E-2</v>
       </c>
-      <c r="K28">
-        <v>6</v>
-      </c>
-      <c r="L28">
-        <f t="shared" si="13"/>
-        <v>0.3125</v>
-      </c>
-      <c r="M28">
-        <f t="shared" si="14"/>
-        <v>0.328125</v>
-      </c>
-      <c r="N28">
-        <f t="shared" si="2"/>
-        <v>0.3203125</v>
-      </c>
-      <c r="O28">
-        <f t="shared" si="15"/>
-        <v>9.4877610051344874E-3</v>
-      </c>
-      <c r="P28">
-        <f t="shared" si="3"/>
-        <v>-4.0422049298882712E-2</v>
-      </c>
-      <c r="Q28">
-        <f t="shared" si="4"/>
-        <v>-1.5489782308668598E-2</v>
-      </c>
-      <c r="T28">
-        <v>6</v>
-      </c>
-      <c r="U28">
-        <f t="shared" si="16"/>
-        <v>1.765625</v>
-      </c>
-      <c r="V28">
-        <f t="shared" si="17"/>
-        <v>1.78125</v>
-      </c>
-      <c r="W28">
-        <f t="shared" si="5"/>
-        <v>1.7734375</v>
-      </c>
-      <c r="X28">
-        <f t="shared" si="18"/>
-        <v>-8.2085517878812908E-2</v>
-      </c>
-      <c r="Y28">
-        <f t="shared" si="6"/>
-        <v>5.7561880955994127E-3</v>
-      </c>
-      <c r="Z28">
-        <f t="shared" si="7"/>
-        <v>-3.8498954300466792E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>7</v>
       </c>
       <c r="C29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-1.234375</v>
       </c>
       <c r="D29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>-1.2265625</v>
       </c>
       <c r="E29">
@@ -4346,82 +3919,28 @@
         <v>-1.23046875</v>
       </c>
       <c r="F29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>-2.1290798148916323E-3</v>
       </c>
       <c r="G29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>5.6431254909981021E-2</v>
       </c>
       <c r="H29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>2.7275723191040768E-2</v>
       </c>
-      <c r="K29">
-        <v>7</v>
-      </c>
-      <c r="L29">
-        <f t="shared" si="13"/>
-        <v>0.3125</v>
-      </c>
-      <c r="M29">
-        <f t="shared" si="14"/>
-        <v>0.3203125</v>
-      </c>
-      <c r="N29">
-        <f t="shared" si="2"/>
-        <v>0.31640625</v>
-      </c>
-      <c r="O29">
-        <f t="shared" si="15"/>
-        <v>9.4877610051344874E-3</v>
-      </c>
-      <c r="P29">
-        <f t="shared" si="3"/>
-        <v>-1.5489782308668598E-2</v>
-      </c>
-      <c r="Q29">
-        <f t="shared" si="4"/>
-        <v>-3.006427010124435E-3</v>
-      </c>
-      <c r="T29">
-        <v>7</v>
-      </c>
-      <c r="U29">
-        <f t="shared" si="16"/>
-        <v>1.7734375</v>
-      </c>
-      <c r="V29">
-        <f t="shared" si="17"/>
-        <v>1.78125</v>
-      </c>
-      <c r="W29">
-        <f t="shared" si="5"/>
-        <v>1.77734375</v>
-      </c>
-      <c r="X29">
-        <f t="shared" si="18"/>
-        <v>-3.8498954300466792E-2</v>
-      </c>
-      <c r="Y29">
-        <f t="shared" si="6"/>
-        <v>5.7561880955994127E-3</v>
-      </c>
-      <c r="Z29">
-        <f t="shared" si="7"/>
-        <v>-1.6455143251628002E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>8</v>
       </c>
       <c r="C30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-1.234375</v>
       </c>
       <c r="D30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>-1.23046875</v>
       </c>
       <c r="E30">
@@ -4429,82 +3948,28 @@
         <v>-1.232421875</v>
       </c>
       <c r="F30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>-2.1290798148916323E-3</v>
       </c>
       <c r="G30">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>2.7275723191040768E-2</v>
       </c>
       <c r="H30">
-        <f t="shared" si="12"/>
+        <f t="shared" si="6"/>
         <v>1.2604537666828897E-2</v>
       </c>
-      <c r="K30">
-        <v>8</v>
-      </c>
-      <c r="L30">
-        <f t="shared" si="13"/>
-        <v>0.3125</v>
-      </c>
-      <c r="M30">
-        <f t="shared" si="14"/>
-        <v>0.31640625</v>
-      </c>
-      <c r="N30">
-        <f t="shared" si="2"/>
-        <v>0.314453125</v>
-      </c>
-      <c r="O30">
-        <f t="shared" si="15"/>
-        <v>9.4877610051344874E-3</v>
-      </c>
-      <c r="P30">
-        <f t="shared" si="3"/>
-        <v>-3.006427010124435E-3</v>
-      </c>
-      <c r="Q30">
-        <f t="shared" si="4"/>
-        <v>3.239343334866418E-3</v>
-      </c>
-      <c r="T30">
-        <v>8</v>
-      </c>
-      <c r="U30">
-        <f t="shared" si="16"/>
-        <v>1.77734375</v>
-      </c>
-      <c r="V30">
-        <f t="shared" si="17"/>
-        <v>1.78125</v>
-      </c>
-      <c r="W30">
-        <f t="shared" si="5"/>
-        <v>1.779296875</v>
-      </c>
-      <c r="X30">
-        <f t="shared" si="18"/>
-        <v>-1.6455143251628002E-2</v>
-      </c>
-      <c r="Y30">
-        <f t="shared" si="6"/>
-        <v>5.7561880955994127E-3</v>
-      </c>
-      <c r="Z30">
-        <f t="shared" si="7"/>
-        <v>-5.3704410824852999E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>9</v>
       </c>
       <c r="C31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>-1.234375</v>
       </c>
       <c r="D31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>-1.232421875</v>
       </c>
       <c r="E31">
@@ -4512,414 +3977,144 @@
         <v>-1.2333984375</v>
       </c>
       <c r="F31">
+        <f t="shared" si="4"/>
+        <v>-2.1290798148916323E-3</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="5"/>
+        <v>1.2604537666828897E-2</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="6"/>
+        <v>5.2455400605149194E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>10</v>
+      </c>
+      <c r="C32">
+        <f t="shared" ref="C32:C34" si="7">IF(F31*H31&lt;0,C31,E31)</f>
+        <v>-1.234375</v>
+      </c>
+      <c r="D32">
+        <f t="shared" ref="D32:D34" si="8">IF(F31*H31&lt;0,E31,D31)</f>
+        <v>-1.2333984375</v>
+      </c>
+      <c r="E32">
+        <f t="shared" ref="E32:E34" si="9">(C32+D32)/2</f>
+        <v>-1.23388671875</v>
+      </c>
+      <c r="F32">
+        <f t="shared" ref="F32:F34" si="10">C32^3-(C32^2*EXP(-0.5*C32))-3*C32+1</f>
+        <v>-2.1290798148916323E-3</v>
+      </c>
+      <c r="G32">
+        <f t="shared" ref="G32:G34" si="11">D32^3-(D32^2*EXP(-0.5*D32))-3*D32+1</f>
+        <v>5.2455400605149194E-3</v>
+      </c>
+      <c r="H32">
+        <f t="shared" ref="H32:H34" si="12">E32^3-(E32^2*EXP(-0.5*E32))-3*E32+1</f>
+        <v>1.5601837993290957E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>11</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="7"/>
+        <v>-1.234375</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="8"/>
+        <v>-1.23388671875</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="9"/>
+        <v>-1.234130859375</v>
+      </c>
+      <c r="F33">
         <f t="shared" si="10"/>
         <v>-2.1290798148916323E-3</v>
       </c>
-      <c r="G31">
+      <c r="G33">
         <f t="shared" si="11"/>
-        <v>1.2604537666828897E-2</v>
-      </c>
-      <c r="H31">
+        <v>1.5601837993290957E-3</v>
+      </c>
+      <c r="H33">
         <f t="shared" si="12"/>
-        <v>5.2455400605149194E-3</v>
-      </c>
-      <c r="K31">
-        <v>9</v>
-      </c>
-      <c r="L31">
-        <f t="shared" si="13"/>
-        <v>0.314453125</v>
-      </c>
-      <c r="M31">
-        <f t="shared" si="14"/>
-        <v>0.31640625</v>
-      </c>
-      <c r="N31">
-        <f t="shared" si="2"/>
-        <v>0.3154296875</v>
-      </c>
-      <c r="O31">
-        <f t="shared" si="15"/>
-        <v>3.239343334866418E-3</v>
-      </c>
-      <c r="P31">
-        <f t="shared" si="3"/>
-        <v>-3.006427010124435E-3</v>
-      </c>
-      <c r="Q31">
-        <f t="shared" si="4"/>
-        <v>1.1612344203659752E-4</v>
-      </c>
-      <c r="T31">
-        <v>9</v>
-      </c>
-      <c r="U31">
-        <f t="shared" si="16"/>
-        <v>1.779296875</v>
-      </c>
-      <c r="V31">
-        <f t="shared" si="17"/>
-        <v>1.78125</v>
-      </c>
-      <c r="W31">
-        <f t="shared" si="5"/>
-        <v>1.7802734375</v>
-      </c>
-      <c r="X31">
-        <f t="shared" si="18"/>
-        <v>-5.3704410824852999E-3</v>
-      </c>
-      <c r="Y31">
-        <f t="shared" si="6"/>
-        <v>5.7561880955994127E-3</v>
-      </c>
-      <c r="Z31">
-        <f t="shared" si="7"/>
-        <v>1.8762969750696357E-4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="B32">
-        <v>10</v>
-      </c>
-      <c r="C32">
-        <f t="shared" ref="C32:C34" si="19">IF(F31*H31&lt;0,C31,E31)</f>
-        <v>-1.234375</v>
-      </c>
-      <c r="D32">
-        <f t="shared" ref="D32:D34" si="20">IF(F31*H31&lt;0,E31,D31)</f>
-        <v>-1.2333984375</v>
-      </c>
-      <c r="E32">
-        <f t="shared" ref="E32:E34" si="21">(C32+D32)/2</f>
-        <v>-1.23388671875</v>
-      </c>
-      <c r="F32">
-        <f t="shared" ref="F32:F34" si="22">C32^3-(C32^2*EXP(-0.5*C32))-3*C32+1</f>
-        <v>-2.1290798148916323E-3</v>
-      </c>
-      <c r="G32">
-        <f t="shared" ref="G32:G34" si="23">D32^3-(D32^2*EXP(-0.5*D32))-3*D32+1</f>
-        <v>5.2455400605149194E-3</v>
-      </c>
-      <c r="H32">
-        <f t="shared" ref="H32:H34" si="24">E32^3-(E32^2*EXP(-0.5*E32))-3*E32+1</f>
-        <v>1.5601837993290957E-3</v>
-      </c>
-      <c r="K32">
-        <v>10</v>
-      </c>
-      <c r="L32">
-        <f t="shared" si="13"/>
-        <v>0.3154296875</v>
-      </c>
-      <c r="M32">
-        <f t="shared" si="14"/>
-        <v>0.31640625</v>
-      </c>
-      <c r="N32">
-        <f t="shared" si="2"/>
-        <v>0.31591796875</v>
-      </c>
-      <c r="O32">
-        <f t="shared" si="15"/>
-        <v>1.1612344203659752E-4</v>
-      </c>
-      <c r="P32">
-        <f t="shared" si="3"/>
-        <v>-3.006427010124435E-3</v>
-      </c>
-      <c r="Q32">
-        <f t="shared" si="4"/>
-        <v>-1.4452359395975556E-3</v>
-      </c>
-      <c r="T32">
-        <v>10</v>
-      </c>
-      <c r="U32">
-        <f t="shared" si="16"/>
-        <v>1.779296875</v>
-      </c>
-      <c r="V32">
-        <f t="shared" si="17"/>
-        <v>1.7802734375</v>
-      </c>
-      <c r="W32">
-        <f t="shared" si="5"/>
-        <v>1.77978515625</v>
-      </c>
-      <c r="X32">
-        <f t="shared" si="18"/>
-        <v>-5.3704410824852999E-3</v>
-      </c>
-      <c r="Y32">
-        <f t="shared" si="6"/>
-        <v>1.8762969750696357E-4</v>
-      </c>
-      <c r="Z32">
-        <f t="shared" si="7"/>
-        <v>-2.5927162781558266E-3</v>
-      </c>
-    </row>
-    <row r="33" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B33">
-        <v>11</v>
-      </c>
-      <c r="C33">
-        <f t="shared" si="19"/>
-        <v>-1.234375</v>
-      </c>
-      <c r="D33">
-        <f t="shared" si="20"/>
-        <v>-1.23388671875</v>
-      </c>
-      <c r="E33">
-        <f t="shared" si="21"/>
-        <v>-1.234130859375</v>
-      </c>
-      <c r="F33">
-        <f t="shared" si="22"/>
-        <v>-2.1290798148916323E-3</v>
-      </c>
-      <c r="G33">
-        <f t="shared" si="23"/>
-        <v>1.5601837993290957E-3</v>
-      </c>
-      <c r="H33">
-        <f t="shared" si="24"/>
         <v>-2.8395947701653768E-4</v>
       </c>
-      <c r="K33">
-        <v>11</v>
-      </c>
-      <c r="L33">
-        <f t="shared" si="13"/>
-        <v>0.3154296875</v>
-      </c>
-      <c r="M33">
-        <f t="shared" si="14"/>
-        <v>0.31591796875</v>
-      </c>
-      <c r="N33">
-        <f t="shared" si="2"/>
-        <v>0.315673828125</v>
-      </c>
-      <c r="O33">
-        <f t="shared" si="15"/>
-        <v>1.1612344203659752E-4</v>
-      </c>
-      <c r="P33">
-        <f t="shared" si="3"/>
-        <v>-1.4452359395975556E-3</v>
-      </c>
-      <c r="Q33">
-        <f t="shared" si="4"/>
-        <v>-6.6457722824031507E-4</v>
-      </c>
-      <c r="T33">
-        <v>11</v>
-      </c>
-      <c r="U33">
-        <f t="shared" si="16"/>
-        <v>1.77978515625</v>
-      </c>
-      <c r="V33">
-        <f t="shared" si="17"/>
-        <v>1.7802734375</v>
-      </c>
-      <c r="W33">
-        <f t="shared" si="5"/>
-        <v>1.780029296875</v>
-      </c>
-      <c r="X33">
-        <f t="shared" si="18"/>
-        <v>-2.5927162781558266E-3</v>
-      </c>
-      <c r="Y33">
-        <f t="shared" si="6"/>
-        <v>1.8762969750696357E-4</v>
-      </c>
-      <c r="Z33">
-        <f t="shared" si="7"/>
-        <v>-1.2028709825662176E-3</v>
-      </c>
-    </row>
-    <row r="34" spans="2:26" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>12</v>
       </c>
       <c r="C34">
-        <f t="shared" si="19"/>
+        <f t="shared" si="7"/>
         <v>-1.234130859375</v>
       </c>
       <c r="D34">
-        <f t="shared" si="20"/>
+        <f t="shared" si="8"/>
         <v>-1.23388671875</v>
       </c>
       <c r="E34">
-        <f t="shared" si="21"/>
+        <f t="shared" si="9"/>
         <v>-1.2340087890625</v>
       </c>
       <c r="F34">
-        <f t="shared" si="22"/>
+        <f t="shared" si="10"/>
         <v>-2.8395947701653768E-4</v>
       </c>
       <c r="G34">
-        <f t="shared" si="23"/>
+        <f t="shared" si="11"/>
         <v>1.5601837993290957E-3</v>
       </c>
       <c r="H34">
-        <f t="shared" si="24"/>
+        <f t="shared" si="12"/>
         <v>6.3823427989184722E-4</v>
       </c>
-      <c r="K34">
-        <v>12</v>
-      </c>
-      <c r="L34">
-        <f t="shared" si="13"/>
-        <v>0.3154296875</v>
-      </c>
-      <c r="M34">
-        <f t="shared" si="14"/>
-        <v>0.315673828125</v>
-      </c>
-      <c r="N34">
-        <f t="shared" si="2"/>
-        <v>0.3155517578125</v>
-      </c>
-      <c r="O34">
-        <f t="shared" si="15"/>
-        <v>1.1612344203659752E-4</v>
-      </c>
-      <c r="P34">
-        <f t="shared" si="3"/>
-        <v>-6.6457722824031507E-4</v>
-      </c>
-      <c r="Q34">
-        <f t="shared" si="4"/>
-        <v>-2.7423213053778817E-4</v>
-      </c>
-      <c r="T34">
-        <v>12</v>
-      </c>
-      <c r="U34">
-        <f t="shared" si="16"/>
-        <v>1.780029296875</v>
-      </c>
-      <c r="V34">
-        <f t="shared" si="17"/>
-        <v>1.7802734375</v>
-      </c>
-      <c r="W34">
-        <f t="shared" si="5"/>
-        <v>1.7801513671875</v>
-      </c>
-      <c r="X34">
-        <f t="shared" si="18"/>
-        <v>-1.2028709825662176E-3</v>
-      </c>
-      <c r="Y34">
-        <f t="shared" si="6"/>
-        <v>1.8762969750696357E-4</v>
-      </c>
-      <c r="Z34">
-        <f t="shared" si="7"/>
-        <v>-5.0770257131826924E-4</v>
-      </c>
-    </row>
-    <row r="35" spans="2:26" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>13</v>
       </c>
       <c r="C35">
-        <f t="shared" ref="C35:C36" si="25">IF(F34*H34&lt;0,C34,E34)</f>
+        <f t="shared" ref="C35:C36" si="13">IF(F34*H34&lt;0,C34,E34)</f>
         <v>-1.234130859375</v>
       </c>
       <c r="D35">
-        <f t="shared" ref="D35:D36" si="26">IF(F34*H34&lt;0,E34,D34)</f>
+        <f t="shared" ref="D35:D36" si="14">IF(F34*H34&lt;0,E34,D34)</f>
         <v>-1.2340087890625</v>
       </c>
       <c r="E35">
-        <f t="shared" ref="E35:E36" si="27">(C35+D35)/2</f>
+        <f t="shared" ref="E35" si="15">(C35+D35)/2</f>
         <v>-1.23406982421875</v>
       </c>
       <c r="F35">
-        <f t="shared" ref="F35:F36" si="28">C35^3-(C35^2*EXP(-0.5*C35))-3*C35+1</f>
+        <f t="shared" ref="F35:F36" si="16">C35^3-(C35^2*EXP(-0.5*C35))-3*C35+1</f>
         <v>-2.8395947701653768E-4</v>
       </c>
       <c r="G35">
-        <f t="shared" ref="G35:G36" si="29">D35^3-(D35^2*EXP(-0.5*D35))-3*D35+1</f>
+        <f t="shared" ref="G35:G36" si="17">D35^3-(D35^2*EXP(-0.5*D35))-3*D35+1</f>
         <v>6.3823427989184722E-4</v>
       </c>
       <c r="H35">
-        <f t="shared" ref="H35:H36" si="30">E35^3-(E35^2*EXP(-0.5*E35))-3*E35+1</f>
+        <f t="shared" ref="H35:H36" si="18">E35^3-(E35^2*EXP(-0.5*E35))-3*E35+1</f>
         <v>1.771679328657072E-4</v>
       </c>
-      <c r="K35">
-        <v>13</v>
-      </c>
-      <c r="L35">
-        <f t="shared" si="13"/>
-        <v>0.3154296875</v>
-      </c>
-      <c r="M35">
-        <f t="shared" si="14"/>
-        <v>0.3155517578125</v>
-      </c>
-      <c r="N35" s="6">
-        <f t="shared" si="2"/>
-        <v>0.31549072265625</v>
-      </c>
-      <c r="O35">
-        <f t="shared" si="15"/>
-        <v>1.1612344203659752E-4</v>
-      </c>
-      <c r="P35">
-        <f t="shared" si="3"/>
-        <v>-2.7423213053778817E-4</v>
-      </c>
-      <c r="Q35">
-        <f t="shared" si="4"/>
-        <v>-7.9055652680848354E-5</v>
-      </c>
-      <c r="T35">
-        <v>13</v>
-      </c>
-      <c r="U35">
-        <f t="shared" si="16"/>
-        <v>1.7801513671875</v>
-      </c>
-      <c r="V35">
-        <f t="shared" si="17"/>
-        <v>1.7802734375</v>
-      </c>
-      <c r="W35">
-        <f t="shared" si="5"/>
-        <v>1.78021240234375</v>
-      </c>
-      <c r="X35">
-        <f t="shared" si="18"/>
-        <v>-5.0770257131826924E-4</v>
-      </c>
-      <c r="Y35">
-        <f t="shared" si="6"/>
-        <v>1.8762969750696357E-4</v>
-      </c>
-      <c r="Z35">
-        <f t="shared" si="7"/>
-        <v>-1.6005691981924031E-4</v>
-      </c>
-    </row>
-    <row r="36" spans="2:26" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>14</v>
       </c>
       <c r="C36">
-        <f t="shared" si="25"/>
+        <f t="shared" si="13"/>
         <v>-1.234130859375</v>
       </c>
       <c r="D36">
-        <f t="shared" si="26"/>
+        <f t="shared" si="14"/>
         <v>-1.23406982421875</v>
       </c>
       <c r="E36" s="6">
@@ -4927,283 +4122,1162 @@
         <v>-1.234100341796875</v>
       </c>
       <c r="F36">
+        <f t="shared" si="16"/>
+        <v>-2.8395947701653768E-4</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="17"/>
+        <v>1.771679328657072E-4</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="18"/>
+        <v>-5.3388139001242507E-5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <f t="shared" ref="E40:E53" si="19">(C40+D40)/2</f>
+        <v>0.5</v>
+      </c>
+      <c r="F40">
+        <f>C40^3-(C40^2*EXP(-0.5*C40))-3*C40+1</f>
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <f t="shared" ref="G40:G53" si="20">D40^3-(D40^2*EXP(-0.5*D40))-3*D40+1</f>
+        <v>-1.6065306597126332</v>
+      </c>
+      <c r="H40">
+        <f t="shared" ref="H40:H53" si="21">E40^3-(E40^2*EXP(-0.5*E40))-3*E40+1</f>
+        <v>-0.56970019576785114</v>
+      </c>
+      <c r="I40">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <f t="shared" ref="C41:C53" si="22">IF(F40*H40&lt;0,C40,E40)</f>
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <f t="shared" ref="D41:D53" si="23">IF(F40*H40&lt;0,E40,D40)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="19"/>
+        <v>0.25</v>
+      </c>
+      <c r="F41">
+        <f t="shared" ref="F41:F53" si="24">C41^3-(C41^2*EXP(-0.5*C41))-3*C41+1</f>
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="20"/>
+        <v>-0.56970019576785114</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="21"/>
+        <v>0.2104689435884628</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="22"/>
+        <v>0.25</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="23"/>
+        <v>0.5</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="19"/>
+        <v>0.375</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="24"/>
+        <v>0.2104689435884628</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="20"/>
+        <v>-0.56970019576785114</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="21"/>
+        <v>-0.18884784474411886</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="22"/>
+        <v>0.25</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="23"/>
+        <v>0.375</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="19"/>
+        <v>0.3125</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="24"/>
+        <v>0.2104689435884628</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="20"/>
+        <v>-0.18884784474411886</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="21"/>
+        <v>9.4877610051344874E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>4</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="22"/>
+        <v>0.3125</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="23"/>
+        <v>0.375</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="19"/>
+        <v>0.34375</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="24"/>
+        <v>9.4877610051344874E-3</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="20"/>
+        <v>-0.18884784474411886</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="21"/>
+        <v>-9.0135220394872428E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>5</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="22"/>
+        <v>0.3125</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="23"/>
+        <v>0.34375</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="19"/>
+        <v>0.328125</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="24"/>
+        <v>9.4877610051344874E-3</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="20"/>
+        <v>-9.0135220394872428E-2</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="21"/>
+        <v>-4.0422049298882712E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>6</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="22"/>
+        <v>0.3125</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="23"/>
+        <v>0.328125</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="19"/>
+        <v>0.3203125</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="24"/>
+        <v>9.4877610051344874E-3</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="20"/>
+        <v>-4.0422049298882712E-2</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="21"/>
+        <v>-1.5489782308668598E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B47">
+        <v>7</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="22"/>
+        <v>0.3125</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="23"/>
+        <v>0.3203125</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="19"/>
+        <v>0.31640625</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="24"/>
+        <v>9.4877610051344874E-3</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="20"/>
+        <v>-1.5489782308668598E-2</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="21"/>
+        <v>-3.006427010124435E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <v>8</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="22"/>
+        <v>0.3125</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="23"/>
+        <v>0.31640625</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="19"/>
+        <v>0.314453125</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="24"/>
+        <v>9.4877610051344874E-3</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="20"/>
+        <v>-3.006427010124435E-3</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="21"/>
+        <v>3.239343334866418E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B49">
+        <v>9</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="22"/>
+        <v>0.314453125</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="23"/>
+        <v>0.31640625</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="19"/>
+        <v>0.3154296875</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="24"/>
+        <v>3.239343334866418E-3</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="20"/>
+        <v>-3.006427010124435E-3</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="21"/>
+        <v>1.1612344203659752E-4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B50">
+        <v>10</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="22"/>
+        <v>0.3154296875</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="23"/>
+        <v>0.31640625</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="19"/>
+        <v>0.31591796875</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="24"/>
+        <v>1.1612344203659752E-4</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="20"/>
+        <v>-3.006427010124435E-3</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="21"/>
+        <v>-1.4452359395975556E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B51">
+        <v>11</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="22"/>
+        <v>0.3154296875</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="23"/>
+        <v>0.31591796875</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="19"/>
+        <v>0.315673828125</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="24"/>
+        <v>1.1612344203659752E-4</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="20"/>
+        <v>-1.4452359395975556E-3</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="21"/>
+        <v>-6.6457722824031507E-4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B52">
+        <v>12</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="22"/>
+        <v>0.3154296875</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="23"/>
+        <v>0.315673828125</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="19"/>
+        <v>0.3155517578125</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="24"/>
+        <v>1.1612344203659752E-4</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="20"/>
+        <v>-6.6457722824031507E-4</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="21"/>
+        <v>-2.7423213053778817E-4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B53">
+        <v>13</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="22"/>
+        <v>0.3154296875</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="23"/>
+        <v>0.3155517578125</v>
+      </c>
+      <c r="E53" s="6">
+        <f t="shared" si="19"/>
+        <v>0.31549072265625</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="24"/>
+        <v>1.1612344203659752E-4</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="20"/>
+        <v>-2.7423213053778817E-4</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="21"/>
+        <v>-7.9055652680848354E-5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I56" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57">
+        <f t="shared" ref="E57:E71" si="25">(C57+D57)/2</f>
+        <v>1.5</v>
+      </c>
+      <c r="F57">
+        <f>C57^3-(C57^2*EXP(-0.5*C57))-3*C57+1</f>
+        <v>-1.6065306597126332</v>
+      </c>
+      <c r="G57">
+        <f t="shared" ref="G57:G71" si="26">D57^3-(D57^2*EXP(-0.5*D57))-3*D57+1</f>
+        <v>1.5284822353142307</v>
+      </c>
+      <c r="H57">
+        <f t="shared" ref="H57:H71" si="27">E57^3-(E57^2*EXP(-0.5*E57))-3*E57+1</f>
+        <v>-1.1878247436672833</v>
+      </c>
+      <c r="I57">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <f t="shared" ref="C58:C71" si="28">IF(F57*H57&lt;0,C57,E57)</f>
+        <v>1.5</v>
+      </c>
+      <c r="D58">
+        <f t="shared" ref="D58:D71" si="29">IF(F57*H57&lt;0,E57,D57)</f>
+        <v>2</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="25"/>
+        <v>1.75</v>
+      </c>
+      <c r="F58">
+        <f t="shared" ref="F58:F71" si="30">C58^3-(C58^2*EXP(-0.5*C58))-3*C58+1</f>
+        <v>-1.1878247436672833</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="26"/>
+        <v>1.5284822353142307</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="27"/>
+        <v>-0.16726493526543162</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59">
         <f t="shared" si="28"/>
-        <v>-2.8395947701653768E-4</v>
-      </c>
-      <c r="G36">
+        <v>1.75</v>
+      </c>
+      <c r="D59">
         <f t="shared" si="29"/>
-        <v>1.771679328657072E-4</v>
-      </c>
-      <c r="H36">
+        <v>2</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="25"/>
+        <v>1.875</v>
+      </c>
+      <c r="F59">
         <f t="shared" si="30"/>
-        <v>-5.3388139001242507E-5</v>
-      </c>
-      <c r="N36" s="24"/>
-      <c r="T36">
+        <v>-0.16726493526543162</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="26"/>
+        <v>1.5284822353142307</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="27"/>
+        <v>0.59005834371437871</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B60">
+        <v>3</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="28"/>
+        <v>1.75</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="29"/>
+        <v>1.875</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="25"/>
+        <v>1.8125</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="30"/>
+        <v>-0.16726493526543162</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="26"/>
+        <v>0.59005834371437871</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="27"/>
+        <v>0.18952259218409928</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B61">
+        <v>4</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="28"/>
+        <v>1.75</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="29"/>
+        <v>1.8125</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="25"/>
+        <v>1.78125</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="30"/>
+        <v>-0.16726493526543162</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="26"/>
+        <v>0.18952259218409928</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="27"/>
+        <v>5.7561880955994127E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B62">
+        <v>5</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="28"/>
+        <v>1.75</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="29"/>
+        <v>1.78125</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="25"/>
+        <v>1.765625</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="30"/>
+        <v>-0.16726493526543162</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="26"/>
+        <v>5.7561880955994127E-3</v>
+      </c>
+      <c r="H62">
+        <f t="shared" si="27"/>
+        <v>-8.2085517878812908E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B63">
+        <v>6</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="28"/>
+        <v>1.765625</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="29"/>
+        <v>1.78125</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="25"/>
+        <v>1.7734375</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="30"/>
+        <v>-8.2085517878812908E-2</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="26"/>
+        <v>5.7561880955994127E-3</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="27"/>
+        <v>-3.8498954300466792E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B64">
+        <v>7</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="28"/>
+        <v>1.7734375</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="29"/>
+        <v>1.78125</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="25"/>
+        <v>1.77734375</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="30"/>
+        <v>-3.8498954300466792E-2</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="26"/>
+        <v>5.7561880955994127E-3</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="27"/>
+        <v>-1.6455143251628002E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B65">
+        <v>8</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="28"/>
+        <v>1.77734375</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="29"/>
+        <v>1.78125</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="25"/>
+        <v>1.779296875</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="30"/>
+        <v>-1.6455143251628002E-2</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="26"/>
+        <v>5.7561880955994127E-3</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="27"/>
+        <v>-5.3704410824852999E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B66">
+        <v>9</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="28"/>
+        <v>1.779296875</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="29"/>
+        <v>1.78125</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="25"/>
+        <v>1.7802734375</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="30"/>
+        <v>-5.3704410824852999E-3</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="26"/>
+        <v>5.7561880955994127E-3</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="27"/>
+        <v>1.8762969750696357E-4</v>
+      </c>
+    </row>
+    <row r="67" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B67">
+        <v>10</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="28"/>
+        <v>1.779296875</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="29"/>
+        <v>1.7802734375</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="25"/>
+        <v>1.77978515625</v>
+      </c>
+      <c r="F67">
+        <f t="shared" si="30"/>
+        <v>-5.3704410824852999E-3</v>
+      </c>
+      <c r="G67">
+        <f t="shared" si="26"/>
+        <v>1.8762969750696357E-4</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="27"/>
+        <v>-2.5927162781558266E-3</v>
+      </c>
+    </row>
+    <row r="68" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B68">
+        <v>11</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="28"/>
+        <v>1.77978515625</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="29"/>
+        <v>1.7802734375</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="25"/>
+        <v>1.780029296875</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="30"/>
+        <v>-2.5927162781558266E-3</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="26"/>
+        <v>1.8762969750696357E-4</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="27"/>
+        <v>-1.2028709825662176E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B69">
+        <v>12</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="28"/>
+        <v>1.780029296875</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="29"/>
+        <v>1.7802734375</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="25"/>
+        <v>1.7801513671875</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="30"/>
+        <v>-1.2028709825662176E-3</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="26"/>
+        <v>1.8762969750696357E-4</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="27"/>
+        <v>-5.0770257131826924E-4</v>
+      </c>
+    </row>
+    <row r="70" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B70">
+        <v>13</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="28"/>
+        <v>1.7801513671875</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="29"/>
+        <v>1.7802734375</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="25"/>
+        <v>1.78021240234375</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="30"/>
+        <v>-5.0770257131826924E-4</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="26"/>
+        <v>1.8762969750696357E-4</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="27"/>
+        <v>-1.6005691981924031E-4</v>
+      </c>
+    </row>
+    <row r="71" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B71">
         <v>14</v>
       </c>
-      <c r="U36">
-        <f t="shared" si="16"/>
+      <c r="C71">
+        <f t="shared" si="28"/>
         <v>1.78021240234375</v>
       </c>
-      <c r="V36">
-        <f t="shared" si="17"/>
+      <c r="D71">
+        <f t="shared" si="29"/>
         <v>1.7802734375</v>
       </c>
-      <c r="W36" s="6">
-        <f t="shared" si="5"/>
+      <c r="E71" s="6">
+        <f t="shared" si="25"/>
         <v>1.780242919921875</v>
       </c>
-      <c r="X36">
-        <f t="shared" si="18"/>
+      <c r="F71">
+        <f t="shared" si="30"/>
         <v>-1.6005691981924031E-4</v>
       </c>
-      <c r="Y36">
-        <f t="shared" si="6"/>
+      <c r="G71">
+        <f t="shared" si="26"/>
         <v>1.8762969750696357E-4</v>
       </c>
-      <c r="Z36">
-        <f t="shared" si="7"/>
+      <c r="H71">
+        <f t="shared" si="27"/>
         <v>1.3781268026313853E-5</v>
       </c>
     </row>
-    <row r="38" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="N38" s="2"/>
-    </row>
-    <row r="39" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B39" s="16" t="s">
+    <row r="72" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="E72" s="25"/>
+    </row>
+    <row r="73" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="E73" s="25"/>
+    </row>
+    <row r="74" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+      <c r="N74" s="2"/>
+    </row>
+    <row r="75" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B75" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="16"/>
-      <c r="N39" s="2"/>
-    </row>
-    <row r="40" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B40" s="13" t="s">
+      <c r="C75" s="17"/>
+      <c r="D75" s="17"/>
+      <c r="E75" s="17"/>
+      <c r="F75" s="17"/>
+      <c r="G75" s="17"/>
+      <c r="H75" s="17"/>
+      <c r="I75" s="17"/>
+      <c r="J75" s="17"/>
+      <c r="N75" s="2"/>
+    </row>
+    <row r="76" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B76" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C40" s="27">
+      <c r="C76" s="16">
         <f>ABS($C$7-E36)/ABS($C$7)*100</f>
         <v>5.7260638368423144E-4</v>
       </c>
-      <c r="D40" s="27"/>
-      <c r="E40" s="13" t="s">
+      <c r="D76" s="16"/>
+      <c r="E76" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F40" s="27">
-        <f>ABS($F$7-N35)/ABS($F$7)*100</f>
+      <c r="F76" s="16">
+        <f>ABS($F$7-E53)/ABS($F$7)*100</f>
         <v>7.8366150987199071E-3</v>
       </c>
-      <c r="G40" s="27"/>
-      <c r="H40" s="13" t="s">
+      <c r="G76" s="16"/>
+      <c r="H76" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="I40" s="27">
-        <f>ABS($I$7-W36)/ABS($I$7)*100</f>
+      <c r="I76" s="16">
+        <f>ABS($I$7-E71)/ABS($I$7)*100</f>
         <v>1.3589298042025023E-4</v>
       </c>
-      <c r="J40" s="27"/>
-      <c r="N40" s="2"/>
-    </row>
-    <row r="41" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B41" s="13"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="27"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="27"/>
-      <c r="J41" s="27"/>
-    </row>
-    <row r="44" spans="2:26" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B44" s="4"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-    </row>
-    <row r="46" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-    </row>
-    <row r="47" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-    </row>
-    <row r="48" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
-      <c r="K48" s="2"/>
-    </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-    </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
-    </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="I55" s="3"/>
-      <c r="J55" s="3"/>
-      <c r="K55" s="3"/>
-      <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
-      <c r="O55" s="3"/>
-    </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="M57" s="2"/>
-    </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="F58" s="2"/>
-      <c r="J58" s="2"/>
-      <c r="M58" s="2"/>
-    </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C59" s="2"/>
-    </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
-      <c r="G62" s="2"/>
-    </row>
-    <row r="63" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B63" s="10"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="12"/>
-      <c r="G63" s="12"/>
-    </row>
-    <row r="64" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B64" s="10"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="12"/>
-      <c r="G64" s="12"/>
-    </row>
-    <row r="67" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B67" s="4"/>
-      <c r="C67" s="4"/>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A71" s="1"/>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
-      <c r="H74" s="3"/>
-      <c r="I74" s="3"/>
-      <c r="J74" s="3"/>
-      <c r="K74" s="3"/>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C80" s="2"/>
-    </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J76" s="16"/>
+      <c r="N76" s="2"/>
+    </row>
+    <row r="77" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B77" s="14"/>
+      <c r="C77" s="16"/>
+      <c r="D77" s="16"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="16"/>
+      <c r="G77" s="16"/>
+      <c r="H77" s="14"/>
+      <c r="I77" s="16"/>
+      <c r="J77" s="16"/>
+    </row>
+    <row r="80" spans="2:14" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B80" s="4"/>
+      <c r="C80" s="13"/>
+      <c r="D80" s="13"/>
+      <c r="E80" s="13"/>
+    </row>
+    <row r="82" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
       <c r="I82" s="2"/>
-    </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
-      <c r="E85" s="2"/>
-      <c r="F85" s="2"/>
-      <c r="G85" s="2"/>
-    </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B86" s="10"/>
-      <c r="C86" s="11"/>
-      <c r="D86" s="11"/>
-      <c r="E86" s="10"/>
-      <c r="F86" s="12"/>
-      <c r="G86" s="12"/>
-    </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B87" s="10"/>
-      <c r="C87" s="11"/>
-      <c r="D87" s="11"/>
-      <c r="E87" s="10"/>
-      <c r="F87" s="12"/>
-      <c r="G87" s="12"/>
-    </row>
-    <row r="90" spans="2:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B90" s="4"/>
+      <c r="J82" s="2"/>
+      <c r="K82" s="2"/>
+    </row>
+    <row r="83" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="I83" s="2"/>
+      <c r="J83" s="2"/>
+      <c r="K83" s="2"/>
+    </row>
+    <row r="84" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="I84" s="2"/>
+      <c r="J84" s="2"/>
+      <c r="K84" s="2"/>
+    </row>
+    <row r="85" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="I85" s="2"/>
+      <c r="J85" s="2"/>
+      <c r="K85" s="2"/>
+    </row>
+    <row r="86" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B86" s="2"/>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
+      <c r="I86" s="2"/>
+      <c r="J86" s="2"/>
+      <c r="K86" s="2"/>
+    </row>
+    <row r="91" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
+      <c r="I91" s="3"/>
+      <c r="J91" s="3"/>
+      <c r="K91" s="3"/>
+      <c r="L91" s="3"/>
+      <c r="M91" s="3"/>
+      <c r="O91" s="3"/>
+    </row>
+    <row r="93" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M93" s="2"/>
+    </row>
+    <row r="94" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="F94" s="2"/>
+      <c r="J94" s="2"/>
+      <c r="M94" s="2"/>
+    </row>
+    <row r="95" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C95" s="2"/>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B98" s="2"/>
+      <c r="C98" s="2"/>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+      <c r="G98" s="2"/>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B99" s="10"/>
+      <c r="C99" s="11"/>
+      <c r="D99" s="11"/>
+      <c r="E99" s="10"/>
+      <c r="F99" s="12"/>
+      <c r="G99" s="12"/>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B100" s="10"/>
+      <c r="C100" s="11"/>
+      <c r="D100" s="11"/>
+      <c r="E100" s="10"/>
+      <c r="F100" s="12"/>
+      <c r="G100" s="12"/>
+    </row>
+    <row r="103" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B103" s="4"/>
+      <c r="C103" s="4"/>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B105" s="2"/>
+      <c r="C105" s="2"/>
+      <c r="D105" s="2"/>
+      <c r="E105" s="2"/>
+      <c r="F105" s="2"/>
+      <c r="G105" s="2"/>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A107" s="1"/>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1"/>
+      <c r="F108" s="1"/>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B110" s="3"/>
+      <c r="C110" s="3"/>
+      <c r="D110" s="3"/>
+      <c r="E110" s="3"/>
+      <c r="H110" s="3"/>
+      <c r="I110" s="3"/>
+      <c r="J110" s="3"/>
+      <c r="K110" s="3"/>
+    </row>
+    <row r="116" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C116" s="2"/>
+    </row>
+    <row r="118" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I118" s="2"/>
+    </row>
+    <row r="121" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B121" s="2"/>
+      <c r="C121" s="2"/>
+      <c r="D121" s="2"/>
+      <c r="E121" s="2"/>
+      <c r="F121" s="2"/>
+      <c r="G121" s="2"/>
+    </row>
+    <row r="122" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B122" s="10"/>
+      <c r="C122" s="11"/>
+      <c r="D122" s="11"/>
+      <c r="E122" s="10"/>
+      <c r="F122" s="12"/>
+      <c r="G122" s="12"/>
+    </row>
+    <row r="123" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B123" s="10"/>
+      <c r="C123" s="11"/>
+      <c r="D123" s="11"/>
+      <c r="E123" s="10"/>
+      <c r="F123" s="12"/>
+      <c r="G123" s="12"/>
+    </row>
+    <row r="126" spans="2:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B126" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C7:D8"/>
+    <mergeCell ref="F7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="C80:E80"/>
     <mergeCell ref="I7:J8"/>
     <mergeCell ref="B6:J6"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F40:G41"/>
-    <mergeCell ref="H40:H41"/>
-    <mergeCell ref="I40:J41"/>
-    <mergeCell ref="B39:J39"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="C76:D77"/>
+    <mergeCell ref="E76:E77"/>
+    <mergeCell ref="F76:G77"/>
+    <mergeCell ref="H76:H77"/>
+    <mergeCell ref="I76:J77"/>
+    <mergeCell ref="B75:J75"/>
     <mergeCell ref="I16:J18"/>
     <mergeCell ref="B16:G16"/>
     <mergeCell ref="B17:G18"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B10:G10"/>
     <mergeCell ref="B11:G12"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="C7:D8"/>
-    <mergeCell ref="F7:G8"/>
-    <mergeCell ref="H7:H8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5231,77 +5305,77 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="18">
         <v>-1.2340932753</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="13" t="s">
+      <c r="D7" s="18"/>
+      <c r="E7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="14">
         <v>0.31546600079999998</v>
       </c>
-      <c r="G7" s="26"/>
-      <c r="H7" s="13" t="s">
+      <c r="G7" s="14"/>
+      <c r="H7" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="14">
         <v>1.7802405007</v>
       </c>
-      <c r="J7" s="26"/>
+      <c r="J7" s="14"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="13"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="15" spans="2:10" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B15" s="4" t="s">
@@ -5309,73 +5383,73 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
@@ -5394,7 +5468,7 @@
       <c r="F26" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G26" s="29"/>
+      <c r="G26" s="1"/>
       <c r="H26" s="8" t="s">
         <v>4</v>
       </c>
@@ -5410,7 +5484,7 @@
       <c r="L26" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="M26" s="29" t="s">
+      <c r="M26" s="1" t="s">
         <v>28</v>
       </c>
       <c r="N26" s="8" t="s">
@@ -5547,10 +5621,7 @@
         <v>7.5550270953337026</v>
       </c>
       <c r="F29" s="2"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="30"/>
-      <c r="K29" s="30"/>
+      <c r="I29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29">
@@ -5577,57 +5648,69 @@
       <c r="C31" s="2"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="27">
+      <c r="C35" s="16">
         <f>ABS($C$7-C29)/ABS($C$7)*100</f>
         <v>1.5545562795588129E-4</v>
       </c>
-      <c r="D35" s="27"/>
-      <c r="E35" s="13" t="s">
+      <c r="D35" s="16"/>
+      <c r="E35" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F35" s="27">
+      <c r="F35" s="16">
         <f>ABS($F$7-I28)/ABS($F$7)*100</f>
         <v>7.3028889444981728E-3</v>
       </c>
-      <c r="G35" s="27"/>
-      <c r="H35" s="13" t="s">
+      <c r="G35" s="16"/>
+      <c r="H35" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="I35" s="27">
+      <c r="I35" s="16">
         <f>ABS($I$7-O29)/ABS($I$7)*100</f>
         <v>7.2440466903906247E-6</v>
       </c>
-      <c r="J35" s="27"/>
+      <c r="J35" s="16"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B36" s="13"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="27"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="27"/>
-      <c r="J36" s="27"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B34:J34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:G36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:J36"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="I17:K20"/>
+    <mergeCell ref="B18:G19"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G23"/>
     <mergeCell ref="B11:G12"/>
     <mergeCell ref="B10:G10"/>
     <mergeCell ref="B6:J6"/>
@@ -5637,18 +5720,6 @@
     <mergeCell ref="F7:G8"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="I7:J8"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="I17:K20"/>
-    <mergeCell ref="B18:G19"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G23"/>
-    <mergeCell ref="B34:J34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:G36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="I35:J36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5676,128 +5747,128 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="18">
         <v>-1.2340932753</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="13" t="s">
+      <c r="D7" s="18"/>
+      <c r="E7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="14">
         <v>0.31546600079999998</v>
       </c>
-      <c r="G7" s="26"/>
-      <c r="H7" s="13" t="s">
+      <c r="G7" s="14"/>
+      <c r="H7" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="14">
         <v>1.7802405007</v>
       </c>
-      <c r="J7" s="26"/>
+      <c r="J7" s="14"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="13"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="15" spans="2:12" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="20"/>
+      <c r="C15" s="21"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
@@ -5854,7 +5925,7 @@
         <v>-2</v>
       </c>
       <c r="D23">
-        <f>C23^3-(C23^2*EXP(-0.5*C23))-3*C23+1</f>
+        <f t="shared" ref="D23:D28" si="0">C23^3-(C23^2*EXP(-0.5*C23))-3*C23+1</f>
         <v>-11.873127313836179</v>
       </c>
       <c r="E23">
@@ -5867,7 +5938,7 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <f>H23^3-(H23^2*EXP(-0.5*H23))-3*H23+1</f>
+        <f t="shared" ref="I23:I28" si="1">H23^3-(H23^2*EXP(-0.5*H23))-3*H23+1</f>
         <v>1</v>
       </c>
       <c r="J23">
@@ -5880,7 +5951,7 @@
         <v>1</v>
       </c>
       <c r="N23">
-        <f>M23^3-(M23^2*EXP(-0.5*M23))-3*M23+1</f>
+        <f t="shared" ref="N23:N28" si="2">M23^3-(M23^2*EXP(-0.5*M23))-3*M23+1</f>
         <v>-1.6065306597126332</v>
       </c>
       <c r="O23">
@@ -5895,7 +5966,7 @@
         <v>-1</v>
       </c>
       <c r="D24">
-        <f>C24^3-(C24^2*EXP(-0.5*C24))-3*C24+1</f>
+        <f t="shared" si="0"/>
         <v>1.3512787292998718</v>
       </c>
       <c r="G24">
@@ -5905,7 +5976,7 @@
         <v>1</v>
       </c>
       <c r="I24">
-        <f>H24^3-(H24^2*EXP(-0.5*H24))-3*H24+1</f>
+        <f t="shared" si="1"/>
         <v>-1.6065306597126332</v>
       </c>
       <c r="L24">
@@ -5915,7 +5986,7 @@
         <v>2</v>
       </c>
       <c r="N24">
-        <f>M24^3-(M24^2*EXP(-0.5*M24))-3*M24+1</f>
+        <f t="shared" si="2"/>
         <v>1.5284822353142307</v>
       </c>
     </row>
@@ -5928,7 +5999,7 @@
         <v>-1.1021806744962459</v>
       </c>
       <c r="D25">
-        <f>C25^3-(C25^2*EXP(-0.5*C25))-3*C25+1</f>
+        <f t="shared" si="0"/>
         <v>0.85975380266030044</v>
       </c>
       <c r="G25">
@@ -5939,7 +6010,7 @@
         <v>0.38365173119055074</v>
       </c>
       <c r="I25">
-        <f>H25^3-(H25^2*EXP(-0.5*H25))-3*H25+1</f>
+        <f t="shared" si="1"/>
         <v>-0.21598297232874852</v>
       </c>
       <c r="L25">
@@ -5950,7 +6021,7 @@
         <v>1.5124478633759708</v>
       </c>
       <c r="N25">
-        <f>M25^3-(M25^2*EXP(-0.5*M25))-3*M25+1</f>
+        <f t="shared" si="2"/>
         <v>-1.1514548029317089</v>
       </c>
     </row>
@@ -5959,22 +6030,22 @@
         <v>3</v>
       </c>
       <c r="C26">
-        <f t="shared" ref="C26" si="0">C25-((D25*(C25-C24))/(D25-D24))</f>
+        <f t="shared" ref="C26" si="3">C25-((D25*(C25-C24))/(D25-D24))</f>
         <v>-1.280910620212633</v>
       </c>
       <c r="D26">
-        <f>C26^3-(C26^2*EXP(-0.5*C26))-3*C26+1</f>
+        <f t="shared" si="0"/>
         <v>-0.37193317628023337</v>
       </c>
       <c r="G26">
         <v>3</v>
       </c>
       <c r="H26">
-        <f t="shared" ref="H26" si="1">H25-((I25*(H25-H24))/(I25-I24))</f>
+        <f t="shared" ref="H26" si="4">H25-((I25*(H25-H24))/(I25-I24))</f>
         <v>0.28791914158221388</v>
       </c>
       <c r="I26">
-        <f>H26^3-(H26^2*EXP(-0.5*H26))-3*H26+1</f>
+        <f t="shared" si="1"/>
         <v>8.8327559886050122E-2</v>
       </c>
       <c r="L26">
@@ -5985,7 +6056,7 @@
         <v>1.7219282509311935</v>
       </c>
       <c r="N26">
-        <f>M26^3-(M26^2*EXP(-0.5*M26))-3*M26+1</f>
+        <f t="shared" si="2"/>
         <v>-0.31368603985038401</v>
       </c>
     </row>
@@ -5993,34 +6064,34 @@
       <c r="B27">
         <v>4</v>
       </c>
-      <c r="C27" s="24">
+      <c r="C27">
         <f>C26-((D26*(C26-C25))/(D26-D25))</f>
         <v>-1.2269394428410332</v>
       </c>
       <c r="D27">
-        <f>C27^3-(C27^2*EXP(-0.5*C27))-3*C27+1</f>
+        <f t="shared" si="0"/>
         <v>5.36286640556769E-2</v>
       </c>
       <c r="G27">
         <v>4</v>
       </c>
-      <c r="H27" s="24">
+      <c r="H27">
         <f>H26-((I26*(H26-H25))/(I26-I25))</f>
         <v>0.31570597492030045</v>
       </c>
       <c r="I27">
-        <f>H27^3-(H27^2*EXP(-0.5*H27))-3*H27+1</f>
+        <f t="shared" si="1"/>
         <v>-7.6737151754913135E-4</v>
       </c>
       <c r="L27">
         <v>4</v>
       </c>
-      <c r="M27" s="24">
+      <c r="M27">
         <f>M26-((N26*(M26-M25))/(N26-N25))</f>
         <v>1.8003640629288087</v>
       </c>
       <c r="N27">
-        <f>M27^3-(M27^2*EXP(-0.5*M27))-3*M27+1</f>
+        <f t="shared" si="2"/>
         <v>0.11686846884061541</v>
       </c>
     </row>
@@ -6028,12 +6099,12 @@
       <c r="B28">
         <v>5</v>
       </c>
-      <c r="C28" s="24">
+      <c r="C28">
         <f>C27-((D27*(C27-C26))/(D27-D26))</f>
         <v>-1.2337408095652354</v>
       </c>
       <c r="D28">
-        <f>C28^3-(C28^2*EXP(-0.5*C28))-3*C28+1</f>
+        <f t="shared" si="0"/>
         <v>2.6618586341129458E-3</v>
       </c>
       <c r="G28">
@@ -6044,18 +6115,18 @@
         <v>0.3154666478998896</v>
       </c>
       <c r="I28">
-        <f>H28^3-(H28^2*EXP(-0.5*H28))-3*H28+1</f>
+        <f t="shared" si="1"/>
         <v>-2.0693652400538554E-6</v>
       </c>
       <c r="L28">
         <v>5</v>
       </c>
-      <c r="M28" s="24">
+      <c r="M28">
         <f>M27-((N27*(M27-M26))/(N27-N26))</f>
         <v>1.7790736732908026</v>
       </c>
       <c r="N28">
-        <f>M28^3-(M28^2*EXP(-0.5*M28))-3*M28+1</f>
+        <f t="shared" si="2"/>
         <v>-6.6393138449374334E-3</v>
       </c>
     </row>
@@ -6064,111 +6135,94 @@
         <v>6</v>
       </c>
       <c r="C29" s="6">
-        <f t="shared" ref="C29" si="2">C28-((D28*(C28-C27))/(D28-D27))</f>
+        <f t="shared" ref="C29" si="5">C28-((D28*(C28-C27))/(D28-D27))</f>
         <v>-1.2340960265851926</v>
       </c>
       <c r="D29">
-        <f t="shared" ref="D29" si="3">C29^3-(C29^2*EXP(-0.5*C29))-3*C29+1</f>
+        <f t="shared" ref="D29" si="6">C29^3-(C29^2*EXP(-0.5*C29))-3*C29+1</f>
         <v>-2.0786386292215298E-5</v>
       </c>
-      <c r="G29" s="30"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
+      <c r="H29" s="2"/>
       <c r="L29">
         <v>6</v>
       </c>
-      <c r="M29" s="24">
-        <f t="shared" ref="M29" si="4">M28-((N28*(M28-M27))/(N28-N27))</f>
+      <c r="M29">
+        <f t="shared" ref="M29" si="7">M28-((N28*(M28-M27))/(N28-N27))</f>
         <v>1.780218164557783</v>
       </c>
       <c r="N29">
-        <f t="shared" ref="N29:N30" si="5">M29^3-(M29^2*EXP(-0.5*M29))-3*M29+1</f>
+        <f t="shared" ref="N29:N30" si="8">M29^3-(M29^2*EXP(-0.5*M29))-3*M29+1</f>
         <v>-1.2723423297789083E-4</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C30" s="24"/>
       <c r="L30">
         <v>7</v>
       </c>
       <c r="M30" s="6">
-        <f t="shared" ref="M30" si="6">M29-((N29*(M29-M28))/(N29-N28))</f>
+        <f t="shared" ref="M30" si="9">M29-((N29*(M29-M28))/(N29-N28))</f>
         <v>1.780240525842838</v>
       </c>
       <c r="N30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.4343420229323556E-7</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C31" s="24"/>
-      <c r="M31" s="24"/>
-    </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="27">
+      <c r="C34" s="16">
         <f>ABS($C$7-C29)/ABS($C$7)*100</f>
         <v>2.2293980913966772E-4</v>
       </c>
-      <c r="D34" s="27"/>
-      <c r="E34" s="13" t="s">
+      <c r="D34" s="16"/>
+      <c r="E34" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F34" s="27">
+      <c r="F34" s="16">
         <f>ABS($F$7-H28)/ABS($F$7)*100</f>
         <v>2.051250809836445E-4</v>
       </c>
-      <c r="G34" s="27"/>
-      <c r="H34" s="13" t="s">
+      <c r="G34" s="16"/>
+      <c r="H34" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="I34" s="27">
+      <c r="I34" s="16">
         <f>ABS($I$7-M30)/ABS($I$7)*100</f>
         <v>1.4123281671156641E-6</v>
       </c>
-      <c r="J34" s="27"/>
+      <c r="J34" s="16"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B35" s="13"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="27"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
     </row>
     <row r="38" spans="2:10" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B38" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B11:G12"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B6:J6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:J8"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="I16:L19"/>
     <mergeCell ref="B17:G17"/>
@@ -6180,6 +6234,15 @@
     <mergeCell ref="H34:H35"/>
     <mergeCell ref="I34:J35"/>
     <mergeCell ref="B33:J33"/>
+    <mergeCell ref="B11:G12"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B6:J6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:J8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6190,7 +6253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C7B6DEE-50FD-4CB9-97D5-BD81BBC974F2}">
   <dimension ref="B6:O102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="M103" sqref="M103"/>
     </sheetView>
   </sheetViews>
@@ -6207,77 +6270,77 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="18">
         <v>-1.2340932753</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="13" t="s">
+      <c r="D7" s="18"/>
+      <c r="E7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="14">
         <v>0.31546600079999998</v>
       </c>
-      <c r="G7" s="26"/>
-      <c r="H7" s="13" t="s">
+      <c r="G7" s="14"/>
+      <c r="H7" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="14">
         <v>1.7802405007</v>
       </c>
-      <c r="J7" s="26"/>
+      <c r="J7" s="14"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="13"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="14" spans="2:10" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B14" s="4" t="s">
@@ -6290,32 +6353,32 @@
       </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C55" s="21" t="s">
+      <c r="C55" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D55" s="21"/>
-      <c r="E55" s="21"/>
-      <c r="H55" s="22" t="s">
+      <c r="D55" s="23"/>
+      <c r="E55" s="23"/>
+      <c r="H55" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="I55" s="22"/>
-      <c r="J55" s="22"/>
-      <c r="M55" s="21" t="s">
+      <c r="I55" s="24"/>
+      <c r="J55" s="24"/>
+      <c r="M55" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="N55" s="21"/>
-      <c r="O55" s="21"/>
+      <c r="N55" s="23"/>
+      <c r="O55" s="23"/>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C56" s="21"/>
-      <c r="D56" s="21"/>
-      <c r="E56" s="21"/>
-      <c r="H56" s="22"/>
-      <c r="I56" s="22"/>
-      <c r="J56" s="22"/>
-      <c r="M56" s="21"/>
-      <c r="N56" s="21"/>
-      <c r="O56" s="21"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="23"/>
+      <c r="H56" s="24"/>
+      <c r="I56" s="24"/>
+      <c r="J56" s="24"/>
+      <c r="M56" s="23"/>
+      <c r="N56" s="23"/>
+      <c r="O56" s="23"/>
     </row>
     <row r="59" spans="2:15" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B59" s="4" t="s">
@@ -6323,32 +6386,32 @@
       </c>
     </row>
     <row r="78" spans="3:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C78" s="21" t="s">
+      <c r="C78" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D78" s="21"/>
-      <c r="E78" s="21"/>
-      <c r="H78" s="22" t="s">
+      <c r="D78" s="23"/>
+      <c r="E78" s="23"/>
+      <c r="H78" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="I78" s="22"/>
-      <c r="J78" s="22"/>
-      <c r="M78" s="21" t="s">
+      <c r="I78" s="24"/>
+      <c r="J78" s="24"/>
+      <c r="M78" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="N78" s="21"/>
-      <c r="O78" s="21"/>
+      <c r="N78" s="23"/>
+      <c r="O78" s="23"/>
     </row>
     <row r="79" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C79" s="21"/>
-      <c r="D79" s="21"/>
-      <c r="E79" s="21"/>
-      <c r="H79" s="22"/>
-      <c r="I79" s="22"/>
-      <c r="J79" s="22"/>
-      <c r="M79" s="21"/>
-      <c r="N79" s="21"/>
-      <c r="O79" s="21"/>
+      <c r="C79" s="23"/>
+      <c r="D79" s="23"/>
+      <c r="E79" s="23"/>
+      <c r="H79" s="24"/>
+      <c r="I79" s="24"/>
+      <c r="J79" s="24"/>
+      <c r="M79" s="23"/>
+      <c r="N79" s="23"/>
+      <c r="O79" s="23"/>
     </row>
     <row r="82" spans="2:2" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B82" s="4" t="s">
@@ -6357,46 +6420,35 @@
     </row>
     <row r="100" spans="3:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="101" spans="3:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C101" s="21" t="s">
+      <c r="C101" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D101" s="21"/>
-      <c r="E101" s="21"/>
-      <c r="H101" s="22" t="s">
+      <c r="D101" s="23"/>
+      <c r="E101" s="23"/>
+      <c r="H101" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="I101" s="22"/>
-      <c r="J101" s="22"/>
-      <c r="M101" s="21" t="s">
+      <c r="I101" s="24"/>
+      <c r="J101" s="24"/>
+      <c r="M101" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="N101" s="21"/>
-      <c r="O101" s="21"/>
+      <c r="N101" s="23"/>
+      <c r="O101" s="23"/>
     </row>
     <row r="102" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C102" s="21"/>
-      <c r="D102" s="21"/>
-      <c r="E102" s="21"/>
-      <c r="H102" s="22"/>
-      <c r="I102" s="22"/>
-      <c r="J102" s="22"/>
-      <c r="M102" s="21"/>
-      <c r="N102" s="21"/>
-      <c r="O102" s="21"/>
+      <c r="C102" s="23"/>
+      <c r="D102" s="23"/>
+      <c r="E102" s="23"/>
+      <c r="H102" s="24"/>
+      <c r="I102" s="24"/>
+      <c r="J102" s="24"/>
+      <c r="M102" s="23"/>
+      <c r="N102" s="23"/>
+      <c r="O102" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C78:E79"/>
-    <mergeCell ref="C101:E102"/>
-    <mergeCell ref="H78:J79"/>
-    <mergeCell ref="M78:O79"/>
-    <mergeCell ref="H101:J102"/>
-    <mergeCell ref="M101:O102"/>
-    <mergeCell ref="M55:O56"/>
-    <mergeCell ref="C55:E56"/>
-    <mergeCell ref="H55:J56"/>
-    <mergeCell ref="B11:G12"/>
-    <mergeCell ref="B10:G10"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:D8"/>
@@ -6404,6 +6456,17 @@
     <mergeCell ref="F7:G8"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="I7:J8"/>
+    <mergeCell ref="M55:O56"/>
+    <mergeCell ref="C55:E56"/>
+    <mergeCell ref="H55:J56"/>
+    <mergeCell ref="B11:G12"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="C78:E79"/>
+    <mergeCell ref="C101:E102"/>
+    <mergeCell ref="H78:J79"/>
+    <mergeCell ref="M78:O79"/>
+    <mergeCell ref="H101:J102"/>
+    <mergeCell ref="M101:O102"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>